<commit_message>
Excel download and excel upload
</commit_message>
<xml_diff>
--- a/public/downloads/Annual Family Gathering Registration .xlsx
+++ b/public/downloads/Annual Family Gathering Registration .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mr.tetteh/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mr.tetteh/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A87D14FB-475F-BD43-9212-4E4159AB4D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593C0757-CA69-AF40-9706-4D284CE7E71F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="7220" windowWidth="27640" windowHeight="16940" xr2:uid="{F51279A6-892D-6A49-BF34-187959DBF804}"/>
+    <workbookView xWindow="4140" yWindow="6440" windowWidth="27640" windowHeight="16940" xr2:uid="{F51279A6-892D-6A49-BF34-187959DBF804}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,27 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>FIRST  NAME</t>
-  </si>
-  <si>
-    <t>LAST NAME</t>
-  </si>
-  <si>
-    <t>OTHER NAMES</t>
-  </si>
-  <si>
-    <t>GENDER</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>CONTACT</t>
   </si>
   <si>
-    <t>CHURCH</t>
+    <t>RESIDENCE</t>
   </si>
   <si>
-    <t>RESIDENCE</t>
+    <t>FULL NAME</t>
+  </si>
+  <si>
+    <t>DENOMINATION</t>
   </si>
 </sst>
 </file>
@@ -435,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467962E7-D28F-4B41-ADDF-0068939007A5}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -446,31 +437,21 @@
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" customWidth="1"/>
-    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>